<commit_message>
LR 3 (1) changed
</commit_message>
<xml_diff>
--- a/LR3/table_1_32.xlsx
+++ b/LR3/table_1_32.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB03F75-18EE-447D-B148-2CD7D1BE25ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A912465-B15E-4441-896B-D8E0E638DE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -689,7 +689,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D38" si="5">D4</f>
+        <f t="shared" ref="D5:D34" si="5">D4</f>
         <v>35.200000000000003</v>
       </c>
       <c r="E5" s="1">
@@ -2009,12 +2009,12 @@
         <v>54</v>
       </c>
       <c r="D35" s="2">
-        <f>D3/3</f>
-        <v>11.733333333333334</v>
+        <f>D3/2</f>
+        <v>17.600000000000001</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>633.6</v>
+        <v>950.40000000000009</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" si="6"/>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="K35" s="1">
         <f t="shared" si="3"/>
-        <v>873.6</v>
+        <v>1190.4000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -2053,12 +2053,12 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" ref="D36:D38" si="9">D4/3</f>
-        <v>11.733333333333334</v>
+        <f t="shared" ref="D36:D38" si="9">D4/2</f>
+        <v>17.600000000000001</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="0"/>
-        <v>627.73333333333335</v>
+        <v>941.6</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" si="6"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="K36" s="1">
         <f t="shared" si="3"/>
-        <v>877.73333333333335</v>
+        <v>1191.5999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -2098,11 +2098,11 @@
       </c>
       <c r="D37" s="2">
         <f t="shared" si="9"/>
-        <v>11.733333333333334</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
-        <v>621.86666666666667</v>
+        <v>932.80000000000007</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="6"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="K37" s="1">
         <f t="shared" si="3"/>
-        <v>881.86666666666667</v>
+        <v>1192.8000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -2142,11 +2142,11 @@
       </c>
       <c r="D38" s="2">
         <f t="shared" si="9"/>
-        <v>11.733333333333334</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
-        <v>616</v>
+        <v>924.00000000000011</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" si="6"/>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="K38" s="1">
         <f t="shared" si="3"/>
-        <v>886</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2178,7 +2178,7 @@
       </c>
       <c r="C40" s="8">
         <f>FLOOR(SUM(K3:K38),1)</f>
-        <v>76397</v>
+        <v>77647</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
LR 3 (1) changed 3
</commit_message>
<xml_diff>
--- a/LR3/table_1_32.xlsx
+++ b/LR3/table_1_32.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDFD0B2-1A07-4C43-9ABE-8F36EBD0745D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00102DB-2B99-4A90-8ABE-70C732CC0EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f>I3</f>
+        <f>$I$3</f>
         <v>10</v>
       </c>
       <c r="J4" s="1">
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f>I4</f>
+        <f>$I$3</f>
         <v>10</v>
       </c>
       <c r="J5" s="1">
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6:I38" si="8">I5</f>
+        <f t="shared" ref="I6:I38" si="8">$I$3</f>
         <v>10</v>
       </c>
       <c r="J6" s="1">
@@ -2169,7 +2169,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="7">
@@ -2178,7 +2178,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="1">
@@ -2187,7 +2187,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C42" s="1">
@@ -2196,7 +2196,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="1">

</xml_diff>

<commit_message>
LR 3 (1) changed 4
</commit_message>
<xml_diff>
--- a/LR3/table_1_32.xlsx
+++ b/LR3/table_1_32.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00102DB-2B99-4A90-8ABE-70C732CC0EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FE779F-883C-4D24-8128-E51D448A6B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
LR 3 (1) changed 6
</commit_message>
<xml_diff>
--- a/LR3/table_1_32.xlsx
+++ b/LR3/table_1_32.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3DDF92B-91B6-4652-9737-3D0DA612E320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A25ECC7-F6EE-4EFD-82C1-3F877687A5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
LR 3 (1) changed 7
</commit_message>
<xml_diff>
--- a/LR3/table_1_32.xlsx
+++ b/LR3/table_1_32.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A25ECC7-F6EE-4EFD-82C1-3F877687A5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2565A0F-8CB0-4516-AED7-316AB1EE0AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -181,7 +181,7 @@
     <t>Максимальная сумма, руб.</t>
   </si>
   <si>
-    <t>Пенни за 1 день, руб.</t>
+    <t>Пени за 1 день, руб.</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>